<commit_message>
Update user stories xlsx
</commit_message>
<xml_diff>
--- a/livrables/originaux/Tondeux_Pierre_2_user_stories_08112024.xlsx
+++ b/livrables/originaux/Tondeux_Pierre_2_user_stories_08112024.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierr\Documents\OpenClassRooms\OpenClassRooms-da-javascript-react\Projets\Tondeux_Pierre_10_learnAtHome_08112024\P10_learnAtHome_OC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierr\Documents\OpenClassRooms\OpenClassRooms-da-javascript-react\Projets\Tondeux_Pierre_10_learnAtHome_08112024\P10_learnAtHome_OC\livrables\originaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4541,6 +4541,1815 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> je suis sur la page du calendrier
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> les évènements sont matérialisés sur le calendrier (rond rouge pour le jour même, cercle gris pour les autres jours, et un rond gris quand il est sélectionné)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> les évènements sont affichés et triés dans l'ordre chronologique
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur un événement
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>si j'ai créé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> l'événement, les détails de l'événement, s'affichent avec toutes les fonctionnalités
+OU
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">si je n'ai pas créé </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l'événement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, les détails de l'événement s'affichent avec des fonctionnalités réduites</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Étant donné que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis connecté
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lorsque</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis sur la page du calendrier
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur "créer un nouvel événement" (ou l'icone "+")
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> une nouvel événement est affichée
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je remplis correctement le formulaire
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j'ajoute un/des participants(s)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur le bouton "créer"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alors </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">l'événement est créé
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> un message est envoyé aux participants pour notifier l'événement
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alors </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l'évènement est matérialisé sur le calendrier (par un cercle gris sur le jour sélectionné)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Alors </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l'évènement est affiché et trié dans la liste par ordre chronologique</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Étant donné que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis connecté
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lorsque</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis sur la page du calendrier
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> les évènements sont matérialisés sur le calendrier (rond rouge pour le jour même, cercle gris pour les autres jours, et un rond gris quand il est sélectionné)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> les évènements sont affichés dans la liste et triés dans l'ordre chronologique
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur un événement
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> si j'ai créé l'événement, les détails de l'événement s'affichent avec toutes les fonctionnalités
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> le bouton "supprimer" est affiché
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur le bouton "supprimer"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> l'événement est supprimé, et retiré du calendrier et de la liste</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Étant donné que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis connecté
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lorsque</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis sur la page du calendrier
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> les évènements sont matérialisés sur le calendrier (rond rouge pour le jour même, cercle gris pour les autres jours, et un rond gris quand il est sélectionné)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> les évènements sont affichés dans la liste et triés dans l'ordre chronologique
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur un événement
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> si j'ai créé l'événement, les détails de l'événement s'affichent avec toutes les fonctionnalités
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> le bouton "Modifier" est affiché
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je modifie les champs du formulaire
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur le bouton "Modifier"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> l'événement est modifié
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> l'évènement est matérialisé sur le calendrier (par un cercle gris sur le jour sélectionné)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> l'évènement est affiché et trié dans la liste par ordre chronologique</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Étant donné que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je ne suis pas inscrit
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lorsque</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis sur la page de connexion
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur "s'inscrire"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis redirigé sur la page d'inscription
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je remplis correctement le formulaire
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur le bouton "s'inscrire"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alors </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">un compte personnel est créé
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> un message de confirmation s'affiche
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je reçois un e-mail de confirmation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Et que </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">je clique sur la confirmation dans l'e-mail
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alors </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">j'accède à mon espace personnel Tableau de bord
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>un tuteur doit m'être attribuer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (un administrateur reçoit un message pour agir)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Étant donné que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je ne suis pas inscrit
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lorsque</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis sur la page de connexion
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur "s'inscrire"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis redirigé sur la page d'inscription
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je remplis correctement le formulaire
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur le bouton "s'inscrire"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alors </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">un compte personnel est créé
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> un message de confirmation s'affiche
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je reçois un e-mail de confirmation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Et que </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">je clique sur la confirmation dans l'e-mail
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alors </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">j'accède à mon espace personnel Tableau de bord
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>un élève doit m'être attribuer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (un administrateur reçoit un message pour agir)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Étant donné que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis inscrit
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lorsque</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis sur la page de connexion
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur "mot de passe oublié"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis redirigé sur la page de mot de passe oublié
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je remplis correctement le formulaire
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur le bouton "mot de passe oublié"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> un message s'affiche me disant qu'un e-mail m'a été envoyé
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je reçois un e-mail de mot de passe oublié
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Et que </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">je clique sur "réinitialiser le mot de passe" dans l'e-mail
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis redirigé sur la page de réinitialisation du mot de passe
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je remplis correctement le formulaire
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Et que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je clique sur le bouton "réinitialiser"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alors </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j'accède à mon espace personnel Tableau de bord</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Étant donné que</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je suis connecté
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lorsque</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> je suis sur la page des tâches
 Et que je sélectionne les taches "</t>
     </r>
@@ -4715,1816 +6524,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> les détails de la tâchent s'affiche avec toutes les fonctionnalités</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Étant donné que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis connecté
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lorsque</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis sur la page du calendrier
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> les évènements sont matérialisés sur le calendrier (rond rouge pour le jour même, cercle gris pour les autres jours, et un rond gris quand il est sélectionné)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> les évènements sont affichés et triés dans l'ordre chronologique
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur un événement
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>si j'ai créé</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> l'événement, les détails de l'événement, s'affichent avec toutes les fonctionnalités
-OU
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">si je n'ai pas créé </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>l'événement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, les détails de l'événement s'affichent avec des fonctionnalités réduites</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Étant donné que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis connecté
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lorsque</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis sur la page du calendrier
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur "créer un nouvel événement" (ou l'icone "+")
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> une nouvel événement est affichée
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je remplis correctement le formulaire
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>j'ajoute un/des participants(s)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur le bouton "créer"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alors </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">l'événement est créé
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> un message est envoyé aux participants pour notifier l'événement
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alors </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>l'évènement est matérialisé sur le calendrier (par un cercle gris sur le jour sélectionné)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Alors </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>l'évènement est affiché et trié dans la liste par ordre chronologique</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Étant donné que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis connecté
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lorsque</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis sur la page du calendrier
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> les évènements sont matérialisés sur le calendrier (rond rouge pour le jour même, cercle gris pour les autres jours, et un rond gris quand il est sélectionné)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> les évènements sont affichés dans la liste et triés dans l'ordre chronologique
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur un événement
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> si j'ai créé l'événement, les détails de l'événement s'affichent avec toutes les fonctionnalités
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> le bouton "supprimer" est affiché
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur le bouton "supprimer"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> l'événement est supprimé, et retiré du calendrier et de la liste</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Étant donné que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis connecté
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lorsque</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis sur la page du calendrier
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> les évènements sont matérialisés sur le calendrier (rond rouge pour le jour même, cercle gris pour les autres jours, et un rond gris quand il est sélectionné)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> les évènements sont affichés dans la liste et triés dans l'ordre chronologique
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur un événement
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> si j'ai créé l'événement, les détails de l'événement s'affichent avec toutes les fonctionnalités
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> le bouton "Modifier" est affiché
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je modifie les champs du formulaire
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur le bouton "Modifier"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> l'événement est modifié
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> l'évènement est matérialisé sur le calendrier (par un cercle gris sur le jour sélectionné)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> l'évènement est affiché et trié dans la liste par ordre chronologique</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Étant donné que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je ne suis pas inscrit
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lorsque</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis sur la page de connexion
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur "s'inscrire"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis redirigé sur la page d'inscription
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je remplis correctement le formulaire
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur le bouton "s'inscrire"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alors </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">un compte personnel est créé
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> un message de confirmation s'affiche
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je reçois un e-mail de confirmation
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Et que </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">je clique sur la confirmation dans l'e-mail
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alors </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">j'accède à mon espace personnel Tableau de bord
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>un tuteur doit m'être attribuer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (un administrateur reçoit un message pour agir)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Étant donné que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je ne suis pas inscrit
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lorsque</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis sur la page de connexion
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur "s'inscrire"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis redirigé sur la page d'inscription
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je remplis correctement le formulaire
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur le bouton "s'inscrire"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alors </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">un compte personnel est créé
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> un message de confirmation s'affiche
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je reçois un e-mail de confirmation
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Et que </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">je clique sur la confirmation dans l'e-mail
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alors </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">j'accède à mon espace personnel Tableau de bord
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>un élève doit m'être attribuer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (un administrateur reçoit un message pour agir)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Étant donné que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis inscrit
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lorsque</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis sur la page de connexion
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur "mot de passe oublié"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis redirigé sur la page de mot de passe oublié
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je remplis correctement le formulaire
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur le bouton "mot de passe oublié"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> un message s'affiche me disant qu'un e-mail m'a été envoyé
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je reçois un e-mail de mot de passe oublié
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Et que </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">je clique sur "réinitialiser le mot de passe" dans l'e-mail
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je suis redirigé sur la page de réinitialisation du mot de passe
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je remplis correctement le formulaire
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Et que</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> je clique sur le bouton "réinitialiser"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alors </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>j'accède à mon espace personnel Tableau de bord</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
+      <t xml:space="preserve"> les détails de la tâche s'affichent avec toutes les fonctionnalités</t>
     </r>
   </si>
 </sst>
@@ -7017,7 +7017,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7060,7 +7060,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -7077,7 +7077,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -7094,7 +7094,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -7114,7 +7114,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
@@ -7131,7 +7131,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
@@ -7182,7 +7182,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
@@ -7559,7 +7559,7 @@
         <v>82</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="180" x14ac:dyDescent="0.25">
@@ -7593,7 +7593,7 @@
         <v>83</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="165" x14ac:dyDescent="0.25">
@@ -7610,7 +7610,7 @@
         <v>90</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="150" x14ac:dyDescent="0.25">
@@ -7627,7 +7627,7 @@
         <v>90</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="195" x14ac:dyDescent="0.25">
@@ -7644,7 +7644,7 @@
         <v>84</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>